<commit_message>
🔥 FINAL FIX: Admin Skills Assessment
</commit_message>
<xml_diff>
--- a/public/skills-assessment-template.xlsx
+++ b/public/skills-assessment-template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,28 +413,55 @@
         <v>skill_name</v>
       </c>
       <c r="D1" t="str">
+        <v>skill_category</v>
+      </c>
+      <c r="E1" t="str">
+        <v>skill_importance</v>
+      </c>
+      <c r="F1" t="str">
         <v>question_text</v>
       </c>
-      <c r="E1" t="str">
+      <c r="G1" t="str">
+        <v>question_type</v>
+      </c>
+      <c r="H1" t="str">
+        <v>difficulty_level</v>
+      </c>
+      <c r="I1" t="str">
         <v>option_1</v>
       </c>
-      <c r="F1" t="str">
+      <c r="J1" t="str">
         <v>option_2</v>
       </c>
-      <c r="G1" t="str">
+      <c r="K1" t="str">
         <v>option_3</v>
       </c>
-      <c r="H1" t="str">
+      <c r="L1" t="str">
         <v>option_4</v>
       </c>
-      <c r="I1" t="str">
+      <c r="M1" t="str">
         <v>correct_answer</v>
       </c>
-      <c r="J1" t="str">
+      <c r="N1" t="str">
         <v>score</v>
       </c>
-      <c r="K1" t="str">
+      <c r="O1" t="str">
+        <v>explanation</v>
+      </c>
+      <c r="P1" t="str">
         <v>course_link</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>course_title</v>
+      </c>
+      <c r="R1" t="str">
+        <v>learning_resource</v>
+      </c>
+      <c r="S1" t="str">
+        <v>estimated_time</v>
+      </c>
+      <c r="T1" t="str">
+        <v>prerequisite_skills</v>
       </c>
     </row>
     <row r="2">
@@ -442,74 +469,66 @@
         <v>Q001</v>
       </c>
       <c r="B2" t="str">
-        <v>Social Media Manager</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="C2" t="str">
-        <v>Content Creation</v>
+        <v>JavaScript</v>
       </c>
       <c r="D2" t="str">
-        <v>คุณใช้เครื่องมือใดในการออกแบบ?</v>
+        <v>Technical</v>
       </c>
       <c r="E2" t="str">
-        <v>Canva</v>
+        <v>Critical</v>
       </c>
       <c r="F2" t="str">
-        <v>Photoshop</v>
+        <v>What is closure in JavaScript?</v>
       </c>
       <c r="G2" t="str">
-        <v>Figma</v>
+        <v>single</v>
       </c>
       <c r="H2" t="str">
-        <v>Illustrator</v>
+        <v>Intermediate</v>
       </c>
       <c r="I2" t="str">
-        <v>2,3,4</v>
-      </c>
-      <c r="J2">
+        <v>Function with access to parent scope</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Loop structure</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Data type</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Operator</v>
+      </c>
+      <c r="M2" t="str">
+        <v>1</v>
+      </c>
+      <c r="N2">
         <v>5</v>
       </c>
-      <c r="K2" t="str">
-        <v>https://example.com/course</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Q002</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Social Media Manager</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Analytics</v>
-      </c>
-      <c r="D3" t="str">
-        <v>เครื่องมือใดที่ใช้วิเคราะห์ Social Media?</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Google Analytics</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Facebook Insights</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Hootsuite</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Buffer</v>
-      </c>
-      <c r="I3" t="str">
-        <v>1,2</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3" t="str">
-        <v>https://example.com/analytics-course</v>
+      <c r="O2" t="str">
+        <v>Closure allows functions to access variables from outer scope</v>
+      </c>
+      <c r="P2" t="str">
+        <v>/courses/javascript-advanced</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>JavaScript Advanced Course</v>
+      </c>
+      <c r="R2" t="str">
+        <v>MDN Web Docs</v>
+      </c>
+      <c r="S2" t="str">
+        <v>40</v>
+      </c>
+      <c r="T2" t="str">
+        <v>JavaScript Basics</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>